<commit_message>
career skill list fixes
</commit_message>
<xml_diff>
--- a/doc/options.xlsx
+++ b/doc/options.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mihaly\Documents\js\cloning-vat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vizha\Documents\shared\cloning-vat\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8200" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8200" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Style" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="Family" sheetId="3" r:id="rId3"/>
     <sheet name="Motivations" sheetId="4" r:id="rId4"/>
     <sheet name="Lifepath" sheetId="5" r:id="rId5"/>
+    <sheet name="Skills" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="411">
   <si>
     <t>Die Roll</t>
   </si>
@@ -973,12 +974,300 @@
   </si>
   <si>
     <t>They like you, you hate them</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Aero Tech</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TECH</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Personal Grooming</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ATTR</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Wardrobe &amp; Style</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Other ATTR skill</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Endurance</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BODY</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Strength Feat</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Swimming</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Other BODY skill</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Interrogation</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> COOL</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Intimidate</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Oratory</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Resist Torture/Drugs</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Streetwise</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Other COOL skill</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Human Perception</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> EMP</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Interview</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Leadership</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Seduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Social</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Persuasion</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Perform</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Other EMP skill</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Accounting</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> INT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Anthropology</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Awareness/Notice</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Biology</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Botany</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Chemistry</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Composition</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Diagnose Illness</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Education</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Expert</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gamble</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Geology</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hide/Evade</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> History</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Know Language</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Library Search</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mathematics</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Physics</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Programming</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Shadow/Track</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Stock Market</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> System Knowledge</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Teaching</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Wilderness Survival</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Zoology</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Other INT skill</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Archery</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> REF</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Athletics</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Brawling</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dance</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dodge &amp; Escape</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Driving</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fencing</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Handgun</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Heavy Weapons</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Martial Art</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Melee</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Motorcycle</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Operate Heavy Machinery</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pilot (Gyro)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pilot (Fixed Wing)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pilot (Dirigible)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pilot (Vect. Trust)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rifle</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Stealth</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Submachinegun</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Other REF skill</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> AV Tech</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Basic Tech</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cryotank Operation</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cyberdeck Deign</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CyberTech</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Demolitions</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Disguise</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Electronics</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Electronic Security</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> First Aid</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Forgery</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gyro Tech</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Paint or Draw</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Photo &amp; Film</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pharmaceuticals</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pick Lock</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pick Pocket</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Play Instrument</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Weaponsmith</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Other TECH skill</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1327,7 +1616,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1502,7 +1791,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1640,7 +1929,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C73"/>
   <sheetViews>
     <sheetView topLeftCell="A54" workbookViewId="0">
@@ -2168,7 +2457,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B63"/>
   <sheetViews>
     <sheetView topLeftCell="A12" workbookViewId="0">
@@ -2629,10 +2918,10 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+    <sheetView topLeftCell="A44" workbookViewId="0">
       <selection activeCell="E59" sqref="E59:E68"/>
     </sheetView>
   </sheetViews>
@@ -3601,4 +3890,1068 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43ECC1FF-4D96-4DBE-AA79-17DBC639E4F0}">
+  <dimension ref="A1:N89"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="24.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>317</v>
+      </c>
+      <c r="C1" t="s">
+        <v>318</v>
+      </c>
+      <c r="E1">
+        <v>23</v>
+      </c>
+      <c r="F1">
+        <v>79</v>
+      </c>
+      <c r="G1">
+        <v>54</v>
+      </c>
+      <c r="H1">
+        <v>49</v>
+      </c>
+      <c r="I1">
+        <v>57</v>
+      </c>
+      <c r="J1">
+        <v>84</v>
+      </c>
+      <c r="K1">
+        <v>85</v>
+      </c>
+      <c r="L1">
+        <v>8</v>
+      </c>
+      <c r="M1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>319</v>
+      </c>
+      <c r="C2" t="s">
+        <v>318</v>
+      </c>
+      <c r="E2" t="str">
+        <f>VLOOKUP(E1,$A$1:$C$89, 2)</f>
+        <v xml:space="preserve"> Awareness/Notice</v>
+      </c>
+      <c r="F2" t="str">
+        <f t="shared" ref="F2:N2" si="0">VLOOKUP(F1,$A$1:$C$89, 2)</f>
+        <v xml:space="preserve"> Forgery</v>
+      </c>
+      <c r="G2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> Handgun</v>
+      </c>
+      <c r="H2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> Brawling</v>
+      </c>
+      <c r="I2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> Melee</v>
+      </c>
+      <c r="J2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> Pick Lock</v>
+      </c>
+      <c r="K2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> Pick Pocket</v>
+      </c>
+      <c r="L2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> Intimidate</v>
+      </c>
+      <c r="M2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> Persuasion</v>
+      </c>
+      <c r="N2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> Personal Grooming</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>320</v>
+      </c>
+      <c r="C3" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>321</v>
+      </c>
+      <c r="C4" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>323</v>
+      </c>
+      <c r="C5" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>324</v>
+      </c>
+      <c r="C6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>325</v>
+      </c>
+      <c r="C7" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>326</v>
+      </c>
+      <c r="C8" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>328</v>
+      </c>
+      <c r="C9" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>329</v>
+      </c>
+      <c r="C10" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>330</v>
+      </c>
+      <c r="C11" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>331</v>
+      </c>
+      <c r="C12" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>332</v>
+      </c>
+      <c r="C13" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>333</v>
+      </c>
+      <c r="C14" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>335</v>
+      </c>
+      <c r="C15" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>336</v>
+      </c>
+      <c r="C16" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>337</v>
+      </c>
+      <c r="C17" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>338</v>
+      </c>
+      <c r="C18" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>339</v>
+      </c>
+      <c r="C19" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>340</v>
+      </c>
+      <c r="C20" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>341</v>
+      </c>
+      <c r="C21" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>342</v>
+      </c>
+      <c r="C22" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>344</v>
+      </c>
+      <c r="C23" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>345</v>
+      </c>
+      <c r="C24" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>346</v>
+      </c>
+      <c r="C25" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>347</v>
+      </c>
+      <c r="C26" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>348</v>
+      </c>
+      <c r="C27" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>349</v>
+      </c>
+      <c r="C28" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>350</v>
+      </c>
+      <c r="C29" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>351</v>
+      </c>
+      <c r="C30" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>352</v>
+      </c>
+      <c r="C31" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>353</v>
+      </c>
+      <c r="C32" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>354</v>
+      </c>
+      <c r="C33" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>355</v>
+      </c>
+      <c r="C34" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>356</v>
+      </c>
+      <c r="C35" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>357</v>
+      </c>
+      <c r="C36" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>358</v>
+      </c>
+      <c r="C37" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>359</v>
+      </c>
+      <c r="C38" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>360</v>
+      </c>
+      <c r="C39" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>361</v>
+      </c>
+      <c r="C40" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>362</v>
+      </c>
+      <c r="C41" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>363</v>
+      </c>
+      <c r="C42" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>364</v>
+      </c>
+      <c r="C43" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>365</v>
+      </c>
+      <c r="C44" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>366</v>
+      </c>
+      <c r="C45" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>367</v>
+      </c>
+      <c r="C46" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>368</v>
+      </c>
+      <c r="C47" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>369</v>
+      </c>
+      <c r="C48" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>371</v>
+      </c>
+      <c r="C49" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>372</v>
+      </c>
+      <c r="C50" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>373</v>
+      </c>
+      <c r="C51" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>374</v>
+      </c>
+      <c r="C52" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>375</v>
+      </c>
+      <c r="C53" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>376</v>
+      </c>
+      <c r="C54" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>377</v>
+      </c>
+      <c r="C55" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>378</v>
+      </c>
+      <c r="C56" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>379</v>
+      </c>
+      <c r="C57" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>380</v>
+      </c>
+      <c r="C58" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>381</v>
+      </c>
+      <c r="C59" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>382</v>
+      </c>
+      <c r="C60" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>383</v>
+      </c>
+      <c r="C61" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>384</v>
+      </c>
+      <c r="C62" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>385</v>
+      </c>
+      <c r="C63" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>386</v>
+      </c>
+      <c r="C64" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>387</v>
+      </c>
+      <c r="C65" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>388</v>
+      </c>
+      <c r="C66" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>389</v>
+      </c>
+      <c r="C67" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>390</v>
+      </c>
+      <c r="C68" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>315</v>
+      </c>
+      <c r="C69" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>391</v>
+      </c>
+      <c r="C70" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>392</v>
+      </c>
+      <c r="C71" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
+        <v>393</v>
+      </c>
+      <c r="C72" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
+        <v>394</v>
+      </c>
+      <c r="C73" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74" t="s">
+        <v>395</v>
+      </c>
+      <c r="C74" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>396</v>
+      </c>
+      <c r="C75" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
+        <v>397</v>
+      </c>
+      <c r="C76" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77" t="s">
+        <v>398</v>
+      </c>
+      <c r="C77" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78" t="s">
+        <v>399</v>
+      </c>
+      <c r="C78" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79" t="s">
+        <v>400</v>
+      </c>
+      <c r="C79" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80" t="s">
+        <v>401</v>
+      </c>
+      <c r="C80" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81" t="s">
+        <v>402</v>
+      </c>
+      <c r="C81" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82" t="s">
+        <v>403</v>
+      </c>
+      <c r="C82" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83" t="s">
+        <v>404</v>
+      </c>
+      <c r="C83" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84" t="s">
+        <v>405</v>
+      </c>
+      <c r="C84" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85" t="s">
+        <v>406</v>
+      </c>
+      <c r="C85" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86" t="s">
+        <v>407</v>
+      </c>
+      <c r="C86" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87" t="s">
+        <v>408</v>
+      </c>
+      <c r="C87" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88" t="s">
+        <v>409</v>
+      </c>
+      <c r="C88" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89" t="s">
+        <v>410</v>
+      </c>
+      <c r="C89" t="s">
+        <v>316</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>